<commit_message>
Getting up to date.
</commit_message>
<xml_diff>
--- a/Model/QIBT_MODEL_LOG.xlsx
+++ b/Model/QIBT_MODEL_LOG.xlsx
@@ -22,23 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>This is a log of the QIBT model as run by C. Holgate. Changes to the model source code are contained within the github repo: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://github.com/chiaraholgate/PartB_Scripts/tree/master/Model</t>
-    </r>
+    <t>This is a log of the QIBT model as run by C. Holgate. Changes to the model source code are contained within the github repo: https://github.com/chiaraholgate/PartB_Scripts/tree/master/Model</t>
   </si>
   <si>
     <t>This spreadsheet is a summary of each experiment. For detailed changes to each model version, see the github repo.</t>
@@ -113,7 +97,8 @@
 In March 2019 two problems were found with these RAIN files. 
 (1) To convert the accumulated hourly rainfall data to 3-hourly rainfall totals, accumulated rainfall in timestep 1 was subtracted from accumulated rainfall at time2=timestep 1+3. The last day of month was taking the first timestep of the next month for all "time2" of that day, when it should have only been taking "time2" as the next day for the last period of the last day of the month. 
 (2) The NARCliM model used a rainfall bucket of 1000mm. A rainfall bucket is used to prevent loss of numerical precision in the accumulated rainfall totals over the course of a long model simulation (e.g. some simulations may be centuries long). This means that any time a cell's accumulated rainfall total exceeds 1000mm, the cell's value is reset to (value-1000), and then continues to accumulate in successive timesteps. Therefore when converting the hourly accumulated rainfall to 3-hourly rainfall totals in the above step, negative values of rainfall resulted (usually around -1000mm or so). At cells where a negative rainfall total was recorded, the QIBT model would not have back-tracked the rainfall of that day, as the total daily rainfall would have been below the simulation threshold of 2mm/day. 
-Both issues were fixed and the RAIN files re-processed on 14/3/19. Previous RAIN processed files have been moved to /srv/ccrc/data03/z3131380/PartB/NARCliM_postprocess/Erroneous_RAIN/ on the storm servers. The corresponding files on NCI, in /g/data/hh5/tmp/w28/jpe561/back_traj/wrfhrly, were deleted and replaced with the corrected files.</t>
+Both issues were fixed and the RAIN files re-processed on 14/3/19. Previous RAIN processed files have been moved to /srv/ccrc/data03/z3131380/PartB/NARCliM_postprocess/Erroneous_RAIN/ on the storm servers. The corresponding files on NCI, in /g/data/hh5/tmp/w28/jpe561/back_traj/wrfhrly, were deleted and replaced with the corrected files. 
+3 May 2019: Error found and model killed before finishing. Model was reading in wrfout variable “T”, which is perterbation potential temperature. Model expects actual temperature, so we need to convert to actual temperature after loading in the pertebation potential temperature (perterbation temp + 300, then convert from theta to T).</t>
   </si>
   <si>
     <t>/home/603/cxh603/PhD/PartB/Scripts/Model/exp03</t>
@@ -132,6 +117,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,6 +139,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -160,6 +147,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,11 +201,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -244,17 +240,17 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="105.790816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="50.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="102.321428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="49"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,13 +258,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -286,73 +292,74 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="0"/>
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="245.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+    <row r="8" customFormat="false" ht="306.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
         <v>43525</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://github.com/chiaraholgate/PartB_Scripts/tree/master/Model"/>
+    <hyperlink ref="A1" r:id="rId1" display="This is a log of the QIBT model as run by C. Holgate. Changes to the model source code are contained within the github repo: https://github.com/chiaraholgate/PartB_Scripts/tree/master/Model"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>